<commit_message>
UPloaded New Elections Database
</commit_message>
<xml_diff>
--- a/Data/newspaper_closure_data_file.xlsx
+++ b/Data/newspaper_closure_data_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10215"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lauriercloud-my.sharepoint.com/personal/skiss_wlu_ca/Documents/projects_folder/News_deserts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lauriercloud-my.sharepoint.com/personal/skiss_wlu_ca/Documents/projects_folder/News_deserts/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8B75803A-B1E0-2440-B6B5-B591AFFE2427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEED5A73-3C8B-C449-A5E7-06EF7B245C8B}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{8B75803A-B1E0-2440-B6B5-B591AFFE2427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1134177C-CC19-B348-A0C9-5139ADFA6CE5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil3" sheetId="4" r:id="rId1"/>
@@ -2854,8 +2854,8 @@
   <dimension ref="A1:U1096"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16158,7 +16158,7 @@
         <v>0</v>
       </c>
       <c r="B399" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>294</v>
@@ -16193,7 +16193,7 @@
         <v>0</v>
       </c>
       <c r="B400" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>294</v>
@@ -16228,7 +16228,7 @@
         <v>0</v>
       </c>
       <c r="B401" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>294</v>
@@ -16263,7 +16263,7 @@
         <v>0</v>
       </c>
       <c r="B402" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>294</v>
@@ -16298,7 +16298,7 @@
         <v>0</v>
       </c>
       <c r="B403" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>294</v>
@@ -16333,7 +16333,7 @@
         <v>0</v>
       </c>
       <c r="B404" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>294</v>
@@ -16368,7 +16368,7 @@
         <v>0</v>
       </c>
       <c r="B405" s="1">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>294</v>
@@ -16403,7 +16403,7 @@
         <v>0</v>
       </c>
       <c r="B406" s="1">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>294</v>

</xml_diff>